<commit_message>
Switched audio jack to better supplier w/ superior documentation. Updated BOM accordingly.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Library/Mobile Documents/com~apple~CloudDocs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Development/kicad_tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{B446EAB1-EB8E-9848-A267-9C9A00292DD0}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{E8383485-D6DF-2448-9012-FFF37287374D}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="460" windowWidth="19600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-4340" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Description</t>
   </si>
@@ -54,9 +53,6 @@
     <t xml:space="preserve">296-44413-5-ND </t>
   </si>
   <si>
-    <t>LM386</t>
-  </si>
-  <si>
     <t>LM386M-1</t>
   </si>
   <si>
@@ -81,33 +77,9 @@
     <t xml:space="preserve"> RC1206FR-071KL </t>
   </si>
   <si>
-    <t>10k pot</t>
-  </si>
-  <si>
     <t>Bourns</t>
   </si>
   <si>
-    <t xml:space="preserve"> PRS11S-N20F-103B1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PRS11S-N20F-103B1-ND </t>
-  </si>
-  <si>
-    <t>Audio Jack</t>
-  </si>
-  <si>
-    <t>Switchcraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 35RASMT2BHNTRX </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SC1489-1-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RES SMD 10 OHM 1% 1/2W 1206 </t>
-  </si>
-  <si>
     <t>Stackpole Electronics</t>
   </si>
   <si>
@@ -117,18 +89,12 @@
     <t xml:space="preserve"> RNCP1206FTD10R0CT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve"> CAP CER 0.047UF 25V X7R 1206 </t>
-  </si>
-  <si>
     <t xml:space="preserve">AC1206KRX7R8BB473 </t>
   </si>
   <si>
     <t xml:space="preserve">311-3231-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve"> RES SMD 1K OHM 1% 1/4W 1206 </t>
-  </si>
-  <si>
     <t>404-1046-1-ND</t>
   </si>
   <si>
@@ -204,20 +170,53 @@
     <t>P122428CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">	CAP ALUM 100UF 20% 25V SMD</t>
-  </si>
-  <si>
     <t>EEE-1EA101XP</t>
   </si>
   <si>
     <t>PCE3898CT-ND</t>
+  </si>
+  <si>
+    <t>CAP ALUM 100UF 20% 25V SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 1K OHM 1% 1/4W 1206 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.047UF 25V X7R 1206 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10 OHM 1% 1/2W 1206 </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>DirtyPCBs</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP-3523SJCT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SJ-3523-SMT-TR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN JACK STEREO 3.5MM SMD R/A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC AMP AUDIO PWR .325W AB 8SOIC </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -226,30 +225,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="18"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,20 +251,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,29 +536,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.62109375" customWidth="1"/>
-    <col min="4" max="4" width="16.76953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.82421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -588,13 +571,13 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -609,10 +592,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
       <c r="F3">
         <v>1</v>
       </c>
@@ -620,19 +612,19 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H18" si="0">G3*F3</f>
+        <f t="shared" ref="H3:H6" si="0">G3*F3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -648,322 +640,301 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4.4770000000000003</v>
+      </c>
+      <c r="H5">
+        <f>G5*F5</f>
+        <v>4.4770000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.2290000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1.776</v>
+      </c>
+      <c r="H7">
+        <f>G7*F7</f>
+        <v>1.776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8">
+        <v>232</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="H8">
+        <f>G8*F8</f>
+        <v>0.66800000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1.359</v>
+      </c>
+      <c r="H9">
+        <f>G9*F9</f>
+        <v>1.359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="H10">
+        <f>G10*F10</f>
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.246</v>
+      </c>
+      <c r="H11">
+        <f>G11*F11</f>
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.113</v>
+      </c>
+      <c r="H12">
+        <f>G12*F12</f>
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="H13">
+        <f>G13*F13</f>
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="H14">
+        <f>G14*F14</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1.1619999999999999</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>1.1619999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
+      <c r="H15">
+        <f>G15*F15</f>
         <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0.246</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>0.246</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>4.4770000000000003</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>4.4770000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>0.113</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>0.22600000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1.776</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>1.776</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1">
-        <v>232</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0.66800000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>1.359</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>1.359</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>0.41499999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.95" x14ac:dyDescent="0.2">
-      <c r="H18">
-        <f>SUM(H2:H17)</f>
-        <v>20.393000000000001</v>
+        <f>G16*F16</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="1">
+        <f>SUM(H2:H16)</f>
+        <v>20.459999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>